<commit_message>
📝, File Data Excell rubah judul nama. Uppercase dan tanpa spasi
</commit_message>
<xml_diff>
--- a/restoran.xlsx
+++ b/restoran.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STUFF\1-KULIAH\0.Semester_6\2. AI\KecerdasanBuatan_S6_Fuzzy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F70460-0393-4072-BB16-2DF74823D2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403C5267-0D85-4467-9506-D667EC24A0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A8540245-1FC1-F74E-B528-1186D598F798}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A8540245-1FC1-F74E-B528-1186D598F798}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>harga</t>
+    <t>PELAYANAN</t>
   </si>
   <si>
-    <t>id Pelanggan</t>
+    <t>ID_PELANGGAN</t>
   </si>
   <si>
-    <t>Pelayanan</t>
+    <t>HARGA</t>
   </si>
 </sst>
 </file>
@@ -77,9 +77,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -398,1123 +397,1124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D52A2B-12DF-0F44-A96E-44CDB5481637}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>29</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>42675</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>30</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>45791</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>71</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>34107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>34</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>51772</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>26321</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>50323</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>37</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>31005</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>42</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>54926</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>18</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>48918</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>61</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>37914</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>83</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>44518</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>56</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>33831</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>79</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>35119</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>33079</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>55</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>22346</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>88</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>47217</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>37103</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>23</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>46273</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>81</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>46450</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>32</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>36312</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>43</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>37801</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>99</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>39211</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>77</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>22825</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>11</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>43004</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>94</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>34513</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>10</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>28711</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>53</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>23319</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>39</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>45668</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>58</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>27703</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>6</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>35571</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>19</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>27802</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>60</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>33705</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>73</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>24704</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>14</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>41017</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>87</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>40607</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>64</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>29803</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>72</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>49697</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>22</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>32227</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>17</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>20122</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>57</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>20600</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>68</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>32311</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>98</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>41118</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>74</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>45778</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>49</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>25927</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>48</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>30146</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>38</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>49222</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>2</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>39852</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>91</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>41986</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>67</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>54283</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="1">
         <v>95</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>45874</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>16</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>50127</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="1">
         <v>40</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>24858</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="1">
         <v>4</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>45388</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>51</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>29120</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="1">
         <v>76</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>34027</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="1">
         <v>62</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>34960</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="1">
         <v>65</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>40180</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="1">
         <v>75</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>35311</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="1">
         <v>25</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>31491</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="1">
         <v>13</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>24630</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="1">
         <v>7</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>37513</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="1">
         <v>70</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>40984</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="1">
         <v>15</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>33102</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="1">
         <v>3</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>41103</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="1">
         <v>69</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>45149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="1">
         <v>80</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>20052</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="1">
         <v>8</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>47324</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="1">
         <v>44</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="1">
         <v>40233</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="1">
         <v>85</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="1">
         <v>24551</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="1">
         <v>41</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>45034</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="1">
         <v>26</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>21729</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="1">
         <v>90</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="1">
         <v>38869</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="1">
         <v>50</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="1">
         <v>43751</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="1">
         <v>66</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="1">
         <v>26142</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="1">
         <v>63</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="1">
         <v>44643</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" s="1">
         <v>35</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="1">
         <v>23454</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="1">
         <v>47</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="1">
         <v>25330</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" s="1">
         <v>86</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="1">
         <v>27315</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" s="1">
         <v>92</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="1">
         <v>22360</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" s="1">
         <v>89</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="1">
         <v>22012</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" s="1">
         <v>52</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="1">
         <v>28905</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" s="1">
         <v>28</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="1">
         <v>52995</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" s="1">
         <v>46</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="1">
         <v>49275</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" s="1">
         <v>82</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="1">
         <v>44073</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" s="1">
         <v>45</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="1">
         <v>35507</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" s="1">
         <v>84</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="1">
         <v>29811</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" s="1">
         <v>78</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="1">
         <v>47995</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" s="1">
         <v>100</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="1">
         <v>35304</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" s="1">
         <v>20</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="1">
         <v>43352</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" s="1">
         <v>93</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91" s="1">
         <v>50325</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" s="1">
         <v>59</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="1">
         <v>22726</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" s="1">
         <v>36</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="1">
         <v>40468</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" s="1">
         <v>1</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94" s="1">
         <v>31255</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" s="1">
         <v>97</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95" s="1">
         <v>52973</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" s="1">
         <v>33</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="1">
         <v>49073</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" s="1">
         <v>21</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="1">
         <v>32345</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" s="1">
         <v>24</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98" s="1">
         <v>52788</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" s="1">
         <v>31</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99" s="1">
         <v>36576</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" s="1">
         <v>54</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100" s="1">
         <v>33738</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" s="1">
         <v>96</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101" s="1">
         <v>54721</v>
       </c>
     </row>

</xml_diff>